<commit_message>
new graphics of caps 361
</commit_message>
<xml_diff>
--- a/FRR-KDF17/FRR_KDF17.xlsx
+++ b/FRR-KDF17/FRR_KDF17.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtinoco2\Downloads\Failures-PMI\FRR-KDF17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C6B08E-950E-4882-8801-CD21E0D561AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BE384-CCE8-4B03-8EF7-73591D64E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="0" windowWidth="20784" windowHeight="12240" xr2:uid="{89CA4CFE-68A8-4159-B253-6CA3C061C031}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89CA4CFE-68A8-4159-B253-6CA3C061C031}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,47 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>corrida_id</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>condicion</t>
   </si>
   <si>
-    <t>capsula_361_sublote</t>
-  </si>
-  <si>
-    <t>capsula_730_sublote</t>
-  </si>
-  <si>
-    <t>frr_faltante_361</t>
-  </si>
-  <si>
-    <t>frr_insuficiente_361</t>
-  </si>
-  <si>
-    <t>frr_excesivo_361</t>
-  </si>
-  <si>
-    <t>frr_posicion_361</t>
-  </si>
-  <si>
-    <t>frr_faltante_730</t>
-  </si>
-  <si>
-    <t>frr_insuficiente_730</t>
-  </si>
-  <si>
-    <t>frr_excesivo_730</t>
-  </si>
-  <si>
-    <t>frr_posicion_730</t>
-  </si>
-  <si>
     <t>desperdicio_total</t>
   </si>
   <si>
@@ -110,14 +77,71 @@
     <t>00011365121-1</t>
   </si>
   <si>
-    <t>0001382865-4</t>
+    <t>Filtros_prod</t>
+  </si>
+  <si>
+    <t>FRR_Corrida</t>
+  </si>
+  <si>
+    <t>FRR_Paros</t>
+  </si>
+  <si>
+    <t>FRR_Total</t>
+  </si>
+  <si>
+    <t>inicio</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>ID_cap</t>
+  </si>
+  <si>
+    <t>Sublote</t>
+  </si>
+  <si>
+    <t>frr_faltante</t>
+  </si>
+  <si>
+    <t>frr_insuficiente</t>
+  </si>
+  <si>
+    <t>frr_excesivo</t>
+  </si>
+  <si>
+    <t>frr_posicion</t>
+  </si>
+  <si>
+    <t>15/12/2025  3:45:00 PM</t>
+  </si>
+  <si>
+    <t>Cod_filtro</t>
+  </si>
+  <si>
+    <t>34.C5T3</t>
+  </si>
+  <si>
+    <t>34.C549</t>
+  </si>
+  <si>
+    <t>%FRR_corr</t>
+  </si>
+  <si>
+    <t>%FRR_paros</t>
+  </si>
+  <si>
+    <t>0001382291-2</t>
+  </si>
+  <si>
+    <t>15/12/2025  4:15:00 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +149,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,14 +204,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -166,8 +254,40 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B5512F39-14E6-4E1C-8F47-30729B98A91D}" name="Table2" displayName="Table2" ref="A1:S11" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:S11" xr:uid="{B5512F39-14E6-4E1C-8F47-30729B98A91D}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{0EF67CFC-2D01-49B0-BE61-F80BB9AA3D53}" name="corrida_id"/>
+    <tableColumn id="2" xr3:uid="{8D7E9191-F232-408A-9AFE-78F05100E1A5}" name="inicio" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{22B92C35-C652-43E5-A768-A085CE127D59}" name="Fin" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7BEB7F75-027A-4F38-8A54-49DD50B5B30F}" name="condicion"/>
+    <tableColumn id="5" xr3:uid="{E2BFDA60-8EB6-48E8-B0BE-DA1BE4A76BFD}" name="Sublote"/>
+    <tableColumn id="17" xr3:uid="{2E8E0EEC-E923-4B23-814A-F572B91D3FC4}" name="Cod_filtro"/>
+    <tableColumn id="6" xr3:uid="{C8FFA508-059A-45CD-995E-CE9A3F474242}" name="ID_cap"/>
+    <tableColumn id="7" xr3:uid="{3983087E-5AF4-4E5B-A703-C5FD3FCA742F}" name="frr_faltante"/>
+    <tableColumn id="8" xr3:uid="{0E441D4A-3E76-4847-B964-1D097AC61BC1}" name="frr_insuficiente"/>
+    <tableColumn id="9" xr3:uid="{FF81D4BB-AB75-40DD-8B78-BDA9026B1E3B}" name="frr_excesivo"/>
+    <tableColumn id="10" xr3:uid="{F46344B0-379E-4A27-BB0D-8A2FC8F76E6F}" name="frr_posicion"/>
+    <tableColumn id="11" xr3:uid="{E3E4FE03-E7C8-471A-863D-32F28CEEF165}" name="desperdicio_total"/>
+    <tableColumn id="12" xr3:uid="{036D65DE-7926-4593-A424-DC860AE99B97}" name="duracion_minutos"/>
+    <tableColumn id="13" xr3:uid="{0CABD2B8-033F-438B-A1B7-2523C85E1B83}" name="Filtros_prod"/>
+    <tableColumn id="14" xr3:uid="{83A7CC6F-82E5-4844-9792-4E8125AAE4EE}" name="FRR_Corrida"/>
+    <tableColumn id="15" xr3:uid="{A4E12FD9-8D5A-4AC3-80CB-EE394C547F2A}" name="FRR_Paros"/>
+    <tableColumn id="16" xr3:uid="{A7CB19AF-8B10-4EE5-8A49-02BF5FDE6001}" name="FRR_Total"/>
+    <tableColumn id="18" xr3:uid="{7792B4DF-3521-4BF6-B0F6-E71CAF37D9C1}" name="%FRR_corr" dataDxfId="1">
+      <calculatedColumnFormula>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{0930F5B7-7400-4801-91E9-B7CB32FC18EF}" name="%FRR_paros" dataDxfId="0">
+      <calculatedColumnFormula>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Paros]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -482,258 +602,718 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED04119-FCD4-4D0E-9F1F-E26336F1911A}">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBA8DDB-BB9B-43AA-AAC1-49AE2296E7C7}">
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="6" width="9.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" customWidth="1"/>
+    <col min="12" max="12" width="17.36328125" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" customWidth="1"/>
+    <col min="16" max="16" width="11.6328125" customWidth="1"/>
+    <col min="17" max="17" width="11.08984375" customWidth="1"/>
+    <col min="18" max="18" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>46003.496527777781</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
+      <c r="C2" s="7">
+        <v>46003.017361111109</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2">
+        <v>361</v>
+      </c>
+      <c r="H2">
         <v>140</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>13</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>34</v>
       </c>
-      <c r="J2">
+      <c r="L2">
+        <f>H2+I2+J2+K2</f>
+        <v>187</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="O2">
+        <v>1065</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q9" si="0">O2+P2</f>
+        <v>1065</v>
+      </c>
+      <c r="R2">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>6.9859154929577463E-2</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>46003.496527777781</v>
+      </c>
+      <c r="C3" s="7">
+        <v>46003.017361111109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3">
+        <v>730</v>
+      </c>
+      <c r="H3">
         <v>926</v>
       </c>
-      <c r="K2">
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="J3">
         <v>13</v>
       </c>
-      <c r="M2">
+      <c r="K3">
         <v>34</v>
       </c>
-      <c r="N2">
-        <f>F2+G2+H2+I2+J2+K2+L2+M2</f>
-        <v>1164</v>
-      </c>
-      <c r="O2">
+      <c r="L3">
+        <f>H3+I3+J3+K3</f>
+        <v>977</v>
+      </c>
+      <c r="M3">
         <v>30</v>
       </c>
+      <c r="N3">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="O3">
+        <v>1065</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>1065</v>
+      </c>
+      <c r="R3">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>6.9859154929577463E-2</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>46003.524305555555</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3">
+      <c r="C4" s="7">
+        <v>46003.542361111111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>361</v>
+      </c>
+      <c r="H4">
         <v>163</v>
       </c>
-      <c r="G3">
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="J4">
         <v>11</v>
       </c>
-      <c r="I3">
+      <c r="K4">
         <v>32</v>
       </c>
-      <c r="J3">
+      <c r="L4">
+        <f>H4+I4+J4+K4</f>
+        <v>210</v>
+      </c>
+      <c r="M4">
+        <v>26</v>
+      </c>
+      <c r="N4">
+        <v>63.3</v>
+      </c>
+      <c r="O4">
+        <v>912</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>912</v>
+      </c>
+      <c r="R4">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>6.9407894736842099E-2</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>46004.524305497682</v>
+      </c>
+      <c r="C5" s="7">
+        <v>46003.542361111111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>730</v>
+      </c>
+      <c r="H5">
         <v>623</v>
       </c>
-      <c r="K3">
+      <c r="I5">
         <v>7</v>
       </c>
-      <c r="L3">
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="M3">
+      <c r="K5">
         <v>47</v>
       </c>
-      <c r="N3">
-        <f>F3+G3+H3+I3+J3+K3+L3+M3</f>
-        <v>891</v>
-      </c>
-      <c r="O3">
+      <c r="L5">
+        <f>H5+I5+J5+K5</f>
+        <v>681</v>
+      </c>
+      <c r="M5">
         <v>26</v>
       </c>
+      <c r="N5">
+        <v>63.3</v>
+      </c>
+      <c r="O5">
+        <v>912</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>912</v>
+      </c>
+      <c r="R5">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>6.9407894736842099E-2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>46003.543055555558</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4">
+      <c r="C6" s="7">
+        <v>46003.069444444445</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>361</v>
+      </c>
+      <c r="H6">
         <v>912</v>
       </c>
-      <c r="G4">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="J6">
         <v>315</v>
       </c>
-      <c r="I4">
+      <c r="K6">
         <v>59</v>
       </c>
-      <c r="J4">
+      <c r="L6">
+        <f>Table2[[#This Row],[frr_faltante]]+Table2[[#This Row],[frr_insuficiente]]+Table2[[#This Row],[frr_excesivo]]+Table2[[#This Row],[frr_posicion]]</f>
+        <v>1288</v>
+      </c>
+      <c r="M6">
+        <v>40</v>
+      </c>
+      <c r="N6">
+        <v>48.4</v>
+      </c>
+      <c r="O6">
+        <v>796</v>
+      </c>
+      <c r="P6">
+        <v>1107</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>1903</v>
+      </c>
+      <c r="R6">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>6.0804020100502509E-2</v>
+      </c>
+      <c r="S6">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Paros]]</f>
+        <v>4.372177055103884E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>46003.543055555558</v>
+      </c>
+      <c r="C7" s="7">
+        <v>46003.069444444445</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>730</v>
+      </c>
+      <c r="H7">
         <v>1476</v>
       </c>
-      <c r="K4">
+      <c r="I7">
         <v>8</v>
       </c>
-      <c r="L4">
+      <c r="J7">
         <v>348</v>
       </c>
-      <c r="M4">
+      <c r="K7">
         <v>63</v>
       </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N5" si="0">F4+G4+H4+I4+J4+K4+L4+M4</f>
-        <v>3183</v>
-      </c>
-      <c r="O4">
+      <c r="L7">
+        <f>Table2[[#This Row],[frr_faltante]]+Table2[[#This Row],[frr_insuficiente]]+Table2[[#This Row],[frr_excesivo]]+Table2[[#This Row],[frr_posicion]]</f>
+        <v>1895</v>
+      </c>
+      <c r="M7">
         <v>40</v>
       </c>
+      <c r="N7">
+        <v>48.4</v>
+      </c>
+      <c r="O7">
+        <v>796</v>
+      </c>
+      <c r="P7">
+        <v>1107</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>1903</v>
+      </c>
+      <c r="R7">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>6.0804020100502509E-2</v>
+      </c>
+      <c r="S7">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Paros]]</f>
+        <v>4.372177055103884E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B8" s="1">
         <v>46003.572916666664</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C8" s="7">
+        <v>46003.088888888888</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>361</v>
+      </c>
+      <c r="H8">
+        <v>86</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>33</v>
+      </c>
+      <c r="L8">
+        <f>Table2[[#This Row],[frr_faltante]]+Table2[[#This Row],[frr_insuficiente]]+Table2[[#This Row],[frr_excesivo]]+Table2[[#This Row],[frr_posicion]]</f>
+        <v>122</v>
+      </c>
+      <c r="M8">
         <v>23</v>
       </c>
-      <c r="F5">
-        <v>86</v>
-      </c>
-      <c r="G5">
+      <c r="N8">
+        <v>56.9</v>
+      </c>
+      <c r="O8">
+        <v>275</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+      <c r="R8">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>0.2069090909090909</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>46003.572916666664</v>
+      </c>
+      <c r="C9" s="7">
+        <v>46003.088888888888</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>730</v>
+      </c>
+      <c r="H9">
+        <v>178</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>33</v>
-      </c>
-      <c r="J5">
-        <v>178</v>
-      </c>
-      <c r="K5">
+      <c r="K9">
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <f>Table2[[#This Row],[frr_faltante]]+Table2[[#This Row],[frr_insuficiente]]+Table2[[#This Row],[frr_excesivo]]+Table2[[#This Row],[frr_posicion]]</f>
+        <v>222</v>
+      </c>
+      <c r="M9">
+        <v>23</v>
+      </c>
+      <c r="N9">
+        <v>56.9</v>
+      </c>
+      <c r="O9">
+        <v>275</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+      <c r="R9">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>0.2069090909090909</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>361</v>
+      </c>
+      <c r="H10">
+        <v>125</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <f>Table2[[#This Row],[frr_faltante]]+Table2[[#This Row],[frr_insuficiente]]+Table2[[#This Row],[frr_excesivo]]+Table2[[#This Row],[frr_posicion]]</f>
+        <v>140</v>
+      </c>
+      <c r="M10">
+        <v>30</v>
+      </c>
+      <c r="N10">
+        <v>75.2</v>
+      </c>
+      <c r="O10">
+        <v>191</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f>Table2[[#This Row],[FRR_Corrida]]+Table2[[#This Row],[FRR_Paros]]</f>
+        <v>191</v>
+      </c>
+      <c r="R10">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>0.39371727748691099</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11">
+        <v>307</v>
+      </c>
+      <c r="H11">
+        <v>63</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>40</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>344</v>
-      </c>
-      <c r="O5">
-        <v>23</v>
+      <c r="L11">
+        <f>Table2[[#This Row],[frr_faltante]]+Table2[[#This Row],[frr_insuficiente]]+Table2[[#This Row],[frr_excesivo]]+Table2[[#This Row],[frr_posicion]]</f>
+        <v>74</v>
+      </c>
+      <c r="M11">
+        <v>30</v>
+      </c>
+      <c r="N11">
+        <v>75.2</v>
+      </c>
+      <c r="O11">
+        <v>191</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f>Table2[[#This Row],[FRR_Corrida]]+Table2[[#This Row],[FRR_Paros]]</f>
+        <v>191</v>
+      </c>
+      <c r="R11">
+        <f>Table2[[#This Row],[Filtros_prod]]/Table2[[#This Row],[FRR_Corrida]]</f>
+        <v>0.39371727748691099</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>